<commit_message>
changes to bug reports
</commit_message>
<xml_diff>
--- a/Beecreative-Checklist-BugReports.xlsx
+++ b/Beecreative-Checklist-BugReports.xlsx
@@ -102,219 +102,10 @@
     <t>User able to have one character or 60,000 character long password</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Summary: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Social network icons in footer not linked and user is not navigated to social network pages</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Steps to Reproduce:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- Navigate to: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>https://beecreative.ba/beecreativci/
--</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Scroll down to footer and click on social network icons</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Expected Results: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>User redirected to social network pages</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Actual Results: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Page scrolls to top</t>
-    </r>
-  </si>
-  <si>
     <t>Social network icons in footer not linked to social network pages</t>
   </si>
   <si>
     <t>User can enter one-character-long phone number, city name, postcode in their personal profile page</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Summary: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Alignement issues on iPad and iPad Pro</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Steps to Reproduce:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- Navigate to: https://beecreative.ba/beecreativci/
-- observe alignment of elements</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Expected Results: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>All web elements align perfectly</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Actual Results: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Elements are not aligned</t>
-    </r>
   </si>
   <si>
     <r>
@@ -464,7 +255,124 @@
     </r>
   </si>
   <si>
-    <t>Landing page does not load correctly on Internet Explorer 11</t>
+    <t>Note</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Summary: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A password can be made up of a single character, but also an infinite number of characters</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Steps to Reproduce:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Navigate to: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://beecreative.ba/beecreativci/
+-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Log in as a freelancer
+- Navigate to 'Promijeni sifru' in left hand side menu
+- add current password, enter 'a' as new password, confirm | enter lorem ipsum text of 60,000&gt; characters as password, confirm</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Expected Results: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User informed that password size must not be over/under certain amount of characters</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Actual Results: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User is able to have a one letter or 60,000 character long password</t>
+    </r>
   </si>
   <si>
     <r>
@@ -602,7 +510,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Confirmation link not available in inbox including: Focused, Other or Junk Mail
+      <t>Confirmation link not available in hotmail inbox including: Focused, Other or Junk Mail
 When attempt to resend email is made, no email is ever received</t>
     </r>
   </si>
@@ -720,7 +628,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>User informed that file size exceeds allowed amount or file able to upload</t>
+      <t>User informed that file size exceeds allowed amount or file able to upload or file type is not permitted</t>
     </r>
     <r>
       <rPr>
@@ -742,7 +650,122 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Upload attempts until ERR_CACHE_MISS error appears</t>
+      <t>Upload attempts for extended periods of time until ERR_CACHE_MISS error appears</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Summary: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Social network icons in footer not linked and user is not navigated to social network pages</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Steps to Reproduce:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Navigate to: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://beecreative.ba/beecreativci/
+-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Scroll down to footer and click on social network icons</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Expected Results: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User redirected to social network pages</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Actual Results: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Social network icons in footer are not linked to social network pages</t>
     </r>
   </si>
   <si>
@@ -859,7 +882,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>User can enter any sort of information in all text fields</t>
+      <t>User can enter enter one-character-long phone number, city name, postcode etc. in their personal profile page, no validation of information created</t>
     </r>
   </si>
   <si>
@@ -874,7 +897,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Elements appear extremely large when page opened with Internet Explorer 11</t>
+      <t>Alignement issues on iPad and iPad Pro</t>
     </r>
     <r>
       <rPr>
@@ -897,6 +920,100 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>- Navigate to: https://beecreative.ba/beecreativci/
+- observe alignment of elements</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Expected Results: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All web elements align perfectly</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Actual Results: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Elements are not aligned on iPad and iPad Pro</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Summary: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Elements appear extremely large when page opened with Internet Explorer 11</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Steps to Reproduce:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>- Navigate to: https://beecreative.ba
 - observe elements</t>
     </r>
@@ -931,7 +1048,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Page loads in same format as on other browsers</t>
+      <t>Page loads in similar format to other browsers</t>
     </r>
     <r>
       <rPr>
@@ -953,128 +1070,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>'Dali su nam povjerenje' logos are loaded accross the screen</t>
-    </r>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Summary: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A password can be made up of a single character, but also an infinite number of characters</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Steps to Reproduce:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- Navigate to: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>https://beecreative.ba/beecreativci/
--</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Log in as a freelancer
-- Navigate to 'Promijeni sifru' in left hand side menu
-- add current password, enter 'a' as new password, confirm | enter lorem ipsum text of 60,000&gt; characters as password, confirm</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Expected Results: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>User informed that password size must not be over/under certain amount of characters</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Actual Results: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>User is able to have a one letter or 60,000 character long password</t>
-    </r>
+      <t>'Dali su nam povjerenje' logos are loaded accross the screen on Explorer 11</t>
+    </r>
+  </si>
+  <si>
+    <t>Dali su nam povjerenje' logos are loaded accross the screen on Explorer 11</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1229,6 +1229,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1656,12 +1659,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="36.6" x14ac:dyDescent="0.7">
       <c r="A1" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="409.6" x14ac:dyDescent="0.65">
       <c r="A2" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1737,7 +1740,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>13</v>
@@ -1770,7 +1773,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1797,7 +1800,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>3</v>
@@ -1811,7 +1814,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>10</v>
@@ -1825,7 +1828,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N3" s="7" t="s">
         <v>8</v>
@@ -1839,29 +1842,29 @@
         <v>8</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="N4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="115.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="202.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="225" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>9</v>
@@ -1870,7 +1873,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>12</v>
@@ -1878,27 +1881,27 @@
     </row>
     <row r="7" spans="1:14" ht="102" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>32</v>
+      <c r="A8" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>